<commit_message>
proofed from Jims final edits
</commit_message>
<xml_diff>
--- a/word/Table1.xlsx
+++ b/word/Table1.xlsx
@@ -91,9 +91,6 @@
     </r>
   </si>
   <si>
-    <t>Table 1: Characteristics of coastal segments used to evaluate seagrass depth of colonization estimates (see Fig. 2 for spatial distribution).  Year is the date of the seagrass coverage and bathymetric data.  Latitude and longitude are the geographic centers of each segment.  Area and depth values are meters and square kilometers, respectively.  Secchi measurements (m) were obtained from the Florida Department of Environmental Protection's Impaired Waters Rule (IWR) database, update number 40.  Secchi mean and standard errors are based on all observations within the ten years preceding each seagrass survey.</t>
-  </si>
-  <si>
     <t>BB: http://atoll.floridamarine.org/Data/metadata/SDE Current/seagrass bigbend 2006 poly.htm</t>
   </si>
   <si>
@@ -149,12 +146,32 @@
   <si>
     <t>WCB: http://atoll.floridamarine.org/data/metadata/SDE Current/seagrass chotawhatchee 2007 poly.htm</t>
   </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times"/>
+      </rPr>
+      <t>Table 1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Characteristics of coastal segments used to evaluate seagrass depth of colonization estimates (see Fig. 2 for spatial distribution).  Year is the date of the seagrass coverage and bathymetric data.  Latitude and longitude are the geographic centers of each segment.  Area and depth values are square kilometers and meters, respectively.  Secchi measurements (m) were obtained from the Florida Department of Environmental Protection's Impaired Waters Rule (IWR) database, update number 40.  Secchi mean and standard errors are based on all observations within the ten years preceding each seagrass survey</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -189,6 +206,17 @@
       <color theme="1"/>
       <name val="Times"/>
       <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times"/>
     </font>
   </fonts>
   <fills count="2">
@@ -231,7 +259,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -256,6 +284,9 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -552,8 +583,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="126" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
-        <v>13</v>
+      <c r="A1" s="10" t="s">
+        <v>19</v>
       </c>
       <c r="B1" s="9"/>
       <c r="C1" s="9"/>
@@ -730,7 +761,7 @@
     </row>
     <row r="12" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B12" s="8"/>
       <c r="C12" s="8"/>
@@ -739,7 +770,7 @@
     </row>
     <row r="13" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B13" s="8"/>
       <c r="C13" s="8"/>
@@ -748,7 +779,7 @@
     </row>
     <row r="14" spans="1:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B14" s="8"/>
       <c r="C14" s="8"/>
@@ -757,7 +788,7 @@
     </row>
     <row r="15" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B15" s="8"/>
       <c r="C15" s="8"/>
@@ -766,7 +797,7 @@
     </row>
     <row r="16" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B16" s="8"/>
       <c r="C16" s="8"/>
@@ -775,7 +806,7 @@
     </row>
     <row r="17" spans="1:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B17" s="8"/>
       <c r="C17" s="8"/>

</xml_diff>